<commit_message>
atc_less takes atc_codes from swissindex if longer
</commit_message>
<xml_diff>
--- a/test/data/xlsx/Packungen_2014_small.xlsx
+++ b/test/data/xlsx/Packungen_2014_small.xlsx
@@ -13,7 +13,7 @@
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">{#name?}</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0" vbProcedure="false">{#name?}</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_1" vbProcedure="false">Sheet1!$3:$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_1" vbProcedure="false">Sheet1!$A$3:$AMC$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$4:$R$13</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">sheet1!#ref!</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">sheet1!#ref!</definedName>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="62">
   <si>
     <t>* Das Gültigkeitsdatum entspricht den Angaben auf der Zulassungsbescheinigung. Provisorische Zulassungen, ohne Erneuerung des Gültigkeitsdatums, sind vorbehalten . Alle in der Liste aufgeführten Arzneimittel sind zum Zeitpunkt der Aktualisierung der Liste zugelassen.</t>
   </si>
@@ -154,6 +154,9 @@
     <t>globulina equina (immunisé avec tissu conjonctif porcin) 8 mg, propylenglycolum, conserv.: E 216, E 218, excipiens pro suppositorio.</t>
   </si>
   <si>
+    <t>J06</t>
+  </si>
+  <si>
     <t>Aqua ad iniectabilia Amino, Injektionslösung</t>
   </si>
   <si>
@@ -184,31 +187,31 @@
     <t>Trägerlösung</t>
   </si>
   <si>
-    <t>Kovel ad us.vet., Emulsion</t>
+    <t>Activelle, Filmtabletten</t>
   </si>
   <si>
-    <t>Dr. E. Gräub AG</t>
+    <t>Novo Nordisk Pharma AG</t>
   </si>
   <si>
-    <t>QA12AX</t>
+    <t>07.08.6.</t>
   </si>
   <si>
-    <t>Tierarzneimittel</t>
+    <t>G03FA</t>
   </si>
   <si>
-    <t>4 x 480</t>
+    <t>28</t>
   </si>
   <si>
-    <t>g</t>
+    <t>Tablette(n)</t>
   </si>
   <si>
-    <t>calcii chloridum dihydricum, magnesii chloridum hexahydricum</t>
+    <t>estradiolum, norethisteroni acetas</t>
   </si>
   <si>
-    <t>calcii chloridum dihydricum 180 g, magnesii chloridum hexahydricum 3.6 g, aromatica, antiox.: E 311 et E 320, conserv.: E 217, excipiens ad emulsionem pro vase 480 g.</t>
+    <t>estradiolum 1 mg ut estradiolum hemihydricum, norethisteroni acetas 0.5 mg, excipiens pro compresso obducto.</t>
   </si>
   <si>
-    <t>Orales Kalziumpräparat für Rinder</t>
+    <t>Hormonsubstitutionstherapie nach der Menopause</t>
   </si>
 </sst>
 </file>
@@ -319,7 +322,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -440,34 +443,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -485,10 +460,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:14"/>
+  <dimension ref="1:15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="14:14"/>
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -509,10 +484,19 @@
     <col collapsed="false" hidden="false" max="16" min="16" style="2" width="33.1785714285714"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="2" width="36.7908163265306"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="2" width="59.1428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="2" width="6.91836734693878"/>
+    <col collapsed="false" hidden="false" max="1017" min="19" style="2" width="6.91836734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="1018" style="0" width="6.91836734693878"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="44.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1" s="4" customFormat="true" ht="44.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AMD1" s="0"/>
+      <c r="AME1" s="0"/>
+      <c r="AMF1" s="0"/>
+      <c r="AMG1" s="0"/>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
+    </row>
     <row r="2" s="6" customFormat="true" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>0</v>
@@ -529,8 +513,15 @@
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
+      <c r="AMD2" s="0"/>
+      <c r="AME2" s="0"/>
+      <c r="AMF2" s="0"/>
+      <c r="AMG2" s="0"/>
+      <c r="AMH2" s="0"/>
+      <c r="AMI2" s="0"/>
+      <c r="AMJ2" s="0"/>
     </row>
-    <row r="3" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -1550,13 +1541,6 @@
       <c r="AMA3" s="0"/>
       <c r="AMB3" s="0"/>
       <c r="AMC3" s="0"/>
-      <c r="AMD3" s="0"/>
-      <c r="AME3" s="0"/>
-      <c r="AMF3" s="0"/>
-      <c r="AMG3" s="0"/>
-      <c r="AMH3" s="0"/>
-      <c r="AMI3" s="0"/>
-      <c r="AMJ3" s="0"/>
     </row>
     <row r="4" s="21" customFormat="true" ht="63.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
@@ -1613,6 +1597,13 @@
       <c r="R4" s="20" t="s">
         <v>19</v>
       </c>
+      <c r="AMD4" s="0"/>
+      <c r="AME4" s="0"/>
+      <c r="AMF4" s="0"/>
+      <c r="AMG4" s="0"/>
+      <c r="AMH4" s="0"/>
+      <c r="AMI4" s="0"/>
+      <c r="AMJ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="22" t="n">
@@ -2666,13 +2657,6 @@
       <c r="AMA5" s="0"/>
       <c r="AMB5" s="0"/>
       <c r="AMC5" s="0"/>
-      <c r="AMD5" s="0"/>
-      <c r="AME5" s="0"/>
-      <c r="AMF5" s="0"/>
-      <c r="AMG5" s="0"/>
-      <c r="AMH5" s="0"/>
-      <c r="AMI5" s="0"/>
-      <c r="AMJ5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="22" t="n">
@@ -3726,13 +3710,6 @@
       <c r="AMA6" s="0"/>
       <c r="AMB6" s="0"/>
       <c r="AMC6" s="0"/>
-      <c r="AMD6" s="0"/>
-      <c r="AME6" s="0"/>
-      <c r="AMF6" s="0"/>
-      <c r="AMG6" s="0"/>
-      <c r="AMH6" s="0"/>
-      <c r="AMI6" s="0"/>
-      <c r="AMJ6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="22" t="n">
@@ -4786,13 +4763,6 @@
       <c r="AMA7" s="0"/>
       <c r="AMB7" s="0"/>
       <c r="AMC7" s="0"/>
-      <c r="AMD7" s="0"/>
-      <c r="AME7" s="0"/>
-      <c r="AMF7" s="0"/>
-      <c r="AMG7" s="0"/>
-      <c r="AMH7" s="0"/>
-      <c r="AMI7" s="0"/>
-      <c r="AMJ7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="22" t="n">
@@ -5846,13 +5816,6 @@
       <c r="AMA8" s="0"/>
       <c r="AMB8" s="0"/>
       <c r="AMC8" s="0"/>
-      <c r="AMD8" s="0"/>
-      <c r="AME8" s="0"/>
-      <c r="AMF8" s="0"/>
-      <c r="AMG8" s="0"/>
-      <c r="AMH8" s="0"/>
-      <c r="AMI8" s="0"/>
-      <c r="AMJ8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="n">
@@ -6906,13 +6869,6 @@
       <c r="AMA9" s="0"/>
       <c r="AMB9" s="0"/>
       <c r="AMC9" s="0"/>
-      <c r="AMD9" s="0"/>
-      <c r="AME9" s="0"/>
-      <c r="AMF9" s="0"/>
-      <c r="AMG9" s="0"/>
-      <c r="AMH9" s="0"/>
-      <c r="AMI9" s="0"/>
-      <c r="AMJ9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="n">
@@ -7966,13 +7922,6 @@
       <c r="AMA10" s="0"/>
       <c r="AMB10" s="0"/>
       <c r="AMC10" s="0"/>
-      <c r="AMD10" s="0"/>
-      <c r="AME10" s="0"/>
-      <c r="AMF10" s="0"/>
-      <c r="AMG10" s="0"/>
-      <c r="AMH10" s="0"/>
-      <c r="AMI10" s="0"/>
-      <c r="AMJ10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="n">
@@ -9026,13 +8975,6 @@
       <c r="AMA11" s="0"/>
       <c r="AMB11" s="0"/>
       <c r="AMC11" s="0"/>
-      <c r="AMD11" s="0"/>
-      <c r="AME11" s="0"/>
-      <c r="AMF11" s="0"/>
-      <c r="AMG11" s="0"/>
-      <c r="AMH11" s="0"/>
-      <c r="AMI11" s="0"/>
-      <c r="AMJ11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="n">
@@ -9051,7 +8993,7 @@
         <v>22</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>24</v>
@@ -10086,13 +10028,6 @@
       <c r="AMA12" s="0"/>
       <c r="AMB12" s="0"/>
       <c r="AMC12" s="0"/>
-      <c r="AMD12" s="0"/>
-      <c r="AME12" s="0"/>
-      <c r="AMF12" s="0"/>
-      <c r="AMG12" s="0"/>
-      <c r="AMH12" s="0"/>
-      <c r="AMI12" s="0"/>
-      <c r="AMJ12" s="0"/>
     </row>
     <row r="13" s="26" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="22" t="n">
@@ -10102,19 +10037,19 @@
         <v>1</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H13" s="27" t="n">
         <v>40225</v>
@@ -10129,76 +10064,146 @@
         <v>1</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M13" s="28" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="N13" s="29" t="s">
         <v>27</v>
       </c>
       <c r="O13" s="26" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="P13" s="26" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Q13" s="26" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="R13" s="0"/>
+      <c r="AMD13" s="0"/>
+      <c r="AME13" s="0"/>
+      <c r="AMF13" s="0"/>
+      <c r="AMG13" s="0"/>
+      <c r="AMH13" s="0"/>
+      <c r="AMI13" s="0"/>
+      <c r="AMJ13" s="0"/>
     </row>
-    <row r="14" s="32" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="30" t="n">
-        <v>54709</v>
-      </c>
-      <c r="B14" s="31" t="n">
+    <row r="14" s="26" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="22" t="n">
+        <v>54708</v>
+      </c>
+      <c r="B14" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C14" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14" s="31" t="s">
+      <c r="C14" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="E14" s="0"/>
-      <c r="F14" s="31" t="s">
+      <c r="D14" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G14" s="31" t="s">
+      <c r="E14" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H14" s="33" t="n">
-        <v>35808</v>
-      </c>
-      <c r="I14" s="33" t="n">
-        <v>35808</v>
-      </c>
-      <c r="J14" s="33" t="n">
-        <v>43424</v>
-      </c>
-      <c r="K14" s="34" t="n">
-        <v>13</v>
-      </c>
-      <c r="L14" s="31" t="s">
+      <c r="F14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="M14" s="35" t="s">
+      <c r="G14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H14" s="27" t="n">
+        <v>36144</v>
+      </c>
+      <c r="I14" s="27" t="n">
+        <v>36144</v>
+      </c>
+      <c r="J14" s="27" t="n">
+        <v>43360</v>
+      </c>
+      <c r="K14" s="24" t="n">
+        <v>17</v>
+      </c>
+      <c r="L14" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="N14" s="36" t="s">
+      <c r="M14" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="N14" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="O14" s="32" t="s">
+      <c r="O14" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="P14" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q14" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="R14" s="0"/>
+      <c r="AMD14" s="0"/>
+      <c r="AME14" s="0"/>
+      <c r="AMF14" s="0"/>
+      <c r="AMG14" s="0"/>
+      <c r="AMH14" s="0"/>
+      <c r="AMI14" s="0"/>
+      <c r="AMJ14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="22" t="n">
+        <v>54708</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H15" s="27" t="n">
+        <v>36144</v>
+      </c>
+      <c r="I15" s="27" t="n">
+        <v>36144</v>
+      </c>
+      <c r="J15" s="27" t="n">
+        <v>43360</v>
+      </c>
+      <c r="K15" s="24" t="n">
+        <v>18</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M15" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="P14" s="32" t="s">
+      <c r="N15" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="O15" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="Q14" s="32" t="s">
+      <c r="P15" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="R14" s="0"/>
+      <c r="Q15" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="R15" s="0"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>